<commit_message>
JavaDoc and file structure
Generated the JavaDoc and made the appendix file structure
</commit_message>
<xml_diff>
--- a/Documents/Sprint_Schedule_v3.xlsx
+++ b/Documents/Sprint_Schedule_v3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RaedrimPC\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thanks\Documents\GitHub\Yes_SEP2\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8866194-EA2F-4299-9F68-60CA0EB521BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383A4042-2E59-4E8E-84A9-799A7BC4A3E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9725D131-B2FB-446C-886D-F31B11A9B83D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9725D131-B2FB-446C-886D-F31B11A9B83D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="71">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -61,9 +61,6 @@
     <t xml:space="preserve"> Sprint 2 starts 13:00</t>
   </si>
   <si>
-    <t>Elaboration ends</t>
-  </si>
-  <si>
     <t>Sprint 2 ends 11:50</t>
   </si>
   <si>
@@ -247,10 +244,10 @@
     <t>M</t>
   </si>
   <si>
-    <t>Final sprint (?)</t>
-  </si>
-  <si>
     <t>Final sprint ends</t>
+  </si>
+  <si>
+    <t>Sprint 5 starts 13:00</t>
   </si>
 </sst>
 </file>
@@ -260,7 +257,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -330,6 +327,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -388,13 +396,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -540,7 +548,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -654,27 +662,42 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -992,20 +1015,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B27040C0-9A08-40B2-8D76-5F140A0B567D}">
   <dimension ref="A15:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" topLeftCell="B40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="36" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="24" customWidth="1"/>
-    <col min="5" max="6" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.7265625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" style="36" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" style="24" customWidth="1"/>
+    <col min="5" max="6" width="19.1796875" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C15" s="36" t="s">
         <v>0</v>
       </c>
@@ -1013,12 +1036,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B16" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="51" t="s">
         <v>66</v>
-      </c>
-      <c r="C16" s="38" t="s">
-        <v>67</v>
       </c>
       <c r="D16" s="26">
         <v>20</v>
@@ -1027,7 +1050,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C17" s="37" t="s">
         <v>4</v>
       </c>
@@ -1035,15 +1058,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C18" s="37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D18" s="30">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C19" s="37" t="s">
         <v>5</v>
       </c>
@@ -1051,7 +1074,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C20" s="37" t="s">
         <v>5</v>
       </c>
@@ -1059,15 +1082,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C21" s="37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D21" s="30">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C22" s="37" t="s">
         <v>4</v>
       </c>
@@ -1075,16 +1098,16 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C23" s="38" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D23" s="43">
         <v>27</v>
       </c>
       <c r="E23" s="44"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C24" s="37" t="s">
         <v>4</v>
       </c>
@@ -1092,15 +1115,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C25" s="37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D25" s="30">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C26" s="37" t="s">
         <v>5</v>
       </c>
@@ -1108,7 +1131,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B27" s="23" t="s">
         <v>2</v>
       </c>
@@ -1118,120 +1141,120 @@
       <c r="D27" s="30">
         <v>1</v>
       </c>
-      <c r="G27" s="52"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G27" s="46"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C28" s="37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D28" s="27">
         <v>2</v>
       </c>
-      <c r="G28" s="52"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G28" s="46"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C29" s="37" t="s">
         <v>4</v>
       </c>
       <c r="D29" s="27">
         <v>3</v>
       </c>
-      <c r="G29" s="52"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G29" s="46"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C30" s="38" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D30" s="43">
         <v>4</v>
       </c>
-      <c r="G30" s="52"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="37" t="s">
+      <c r="G30" s="46"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C31" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="30">
+      <c r="D31" s="26">
         <v>5</v>
       </c>
-      <c r="G31" s="52"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G31" s="46"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C32" s="37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D32" s="30">
         <v>6</v>
       </c>
-      <c r="G32" s="52"/>
-    </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G32" s="46"/>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C33" s="37" t="s">
         <v>5</v>
       </c>
       <c r="D33" s="30">
         <v>7</v>
       </c>
-      <c r="G33" s="52"/>
-    </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G33" s="46"/>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C34" s="37" t="s">
         <v>5</v>
       </c>
       <c r="D34" s="27">
         <v>8</v>
       </c>
-      <c r="G34" s="52"/>
-    </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G34" s="46"/>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C35" s="37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D35" s="27">
         <v>9</v>
       </c>
-      <c r="G35" s="52"/>
-    </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G35" s="46"/>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C36" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="26">
+      <c r="D36" s="28">
         <v>10</v>
       </c>
-      <c r="G36" s="52"/>
-    </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C37" s="38" t="s">
-        <v>67</v>
+      <c r="E36" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" s="46"/>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C37" s="39" t="s">
+        <v>66</v>
       </c>
       <c r="D37" s="28">
         <v>11</v>
       </c>
-      <c r="E37" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="F37" s="21" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C38" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="30">
+      <c r="D38" s="28">
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C39" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="D39" s="30">
+        <v>67</v>
+      </c>
+      <c r="D39" s="28">
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C40" s="37" t="s">
         <v>5</v>
       </c>
@@ -1239,7 +1262,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C41" s="37" t="s">
         <v>5</v>
       </c>
@@ -1247,56 +1270,60 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C42" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="D42" s="30">
+        <v>68</v>
+      </c>
+      <c r="D42" s="29">
         <v>16</v>
       </c>
-    </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C43" s="39" t="s">
+      <c r="E42" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C43" s="40" t="s">
         <v>4</v>
       </c>
       <c r="D43" s="29">
         <v>17</v>
       </c>
-      <c r="E43" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="G43" s="35" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G43" s="35"/>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C44" s="40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D44" s="29">
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C45" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="27">
+      <c r="D45" s="29">
         <v>19</v>
       </c>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C46" s="40" t="s">
-        <v>68</v>
-      </c>
-      <c r="D46" s="30">
+        <v>67</v>
+      </c>
+      <c r="D46" s="32">
         <v>20</v>
       </c>
-    </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E46" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F46" s="34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C47" s="37" t="s">
         <v>5</v>
       </c>
@@ -1304,7 +1331,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C48" s="37" t="s">
         <v>5</v>
       </c>
@@ -1312,21 +1339,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C49" s="40" t="s">
-        <v>69</v>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C49" s="41" t="s">
+        <v>68</v>
       </c>
       <c r="D49" s="32">
         <v>23</v>
       </c>
-      <c r="E49" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="F49" s="34" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C50" s="41" t="s">
         <v>4</v>
       </c>
@@ -1334,45 +1355,45 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C51" s="41" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D51" s="32">
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C52" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="D52" s="32">
+      <c r="D52" s="53">
         <v>26</v>
       </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C53" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="D53" s="47">
+      <c r="E52" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52" s="45" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C53" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="D53" s="54">
         <v>27</v>
       </c>
-      <c r="E53" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="F53" s="48" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C54" s="45" t="s">
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C54" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="D54" s="46">
+      <c r="D54" s="52">
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C55" s="37" t="s">
         <v>5</v>
       </c>
@@ -1380,37 +1401,37 @@
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C56" s="45" t="s">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C56" s="56" t="s">
+        <v>68</v>
+      </c>
+      <c r="D56" s="57">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C57" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" s="57">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B58" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C58" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="D58" s="50">
+        <v>1</v>
+      </c>
+      <c r="E58" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="D56" s="46">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C57" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="D57" s="46">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B58" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="C58" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="D58" s="47">
-        <v>1</v>
-      </c>
-      <c r="E58" s="48" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6" ht="21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="59" spans="2:6" ht="21" x14ac:dyDescent="0.5">
       <c r="C59" s="37" t="s">
         <v>4</v>
       </c>
@@ -1418,7 +1439,7 @@
         <v>2</v>
       </c>
       <c r="E59" s="33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1436,283 +1457,283 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="23.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="49" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B1" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="48"/>
+      <c r="D1" s="49"/>
+      <c r="F1" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="51"/>
-      <c r="F1" s="49" t="s">
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="50"/>
-      <c r="H1" s="51"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="D2" s="3"/>
       <c r="F2" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="20"/>
       <c r="I2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B3" s="4" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="G3" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="H3" s="13"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B4" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="H3" s="13"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B5" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B6" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B8" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B9" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="10"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="D10" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="D11" s="13"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B12" s="11" t="s">
         <v>36</v>
-      </c>
-      <c r="D11" s="13"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
-        <v>37</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="13"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B13" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="13"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B14" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="D14" s="16"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B15" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="D14" s="16"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>43</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>44</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B18" s="11" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="11" t="s">
-        <v>46</v>
       </c>
       <c r="C18" s="12"/>
       <c r="D18" s="13"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B19" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="13"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B20" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="12"/>
       <c r="D20" s="13"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="11" t="s">
         <v>49</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>50</v>
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="13"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B22" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B23" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="10"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B24" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C24" s="12"/>
       <c r="D24" s="17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B25" s="11" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="11" t="s">
-        <v>55</v>
       </c>
       <c r="C25" s="12"/>
       <c r="D25" s="13"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B26" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="13"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="C27" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="D27" s="16"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B28" s="11" t="s">
         <v>59</v>
-      </c>
-      <c r="D27" s="16"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="11" t="s">
-        <v>60</v>
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="13"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B29" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="7"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B30" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="10"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B31" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B32" s="18" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="18" t="s">
-        <v>65</v>
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="13"/>

</xml_diff>